<commit_message>
International grosses removed. Row inserts moved. Cleaned activities
</commit_message>
<xml_diff>
--- a/Movie_Data_Template.xlsx
+++ b/Movie_Data_Template.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Documents\UiPath\Group8-300-762-1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Documents\UiPath\Group8-300-762\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{121E5588-187F-4E2E-A420-FC54BD6EF0F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B593F15-13DF-448B-BA04-12630E4500D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" firstSheet="1" activeTab="1" xr2:uid="{D64A0BB7-C040-40A0-96DB-DB75B657400A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D64A0BB7-C040-40A0-96DB-DB75B657400A}"/>
   </bookViews>
   <sheets>
     <sheet name="MovieInfo" sheetId="2" r:id="rId1"/>
-    <sheet name="MovieCrew" sheetId="1" r:id="rId2"/>
+    <sheet name="Director's Highest gross Films" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
   <si>
     <t>Film Title</t>
   </si>
@@ -49,9 +49,6 @@
   </si>
   <si>
     <t>Domestic Gross</t>
-  </si>
-  <si>
-    <t>International Gross</t>
   </si>
   <si>
     <t>Worldwide Gross</t>
@@ -494,23 +491,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CB63AF4-255B-4F4F-A06E-18EAB1273824}">
-  <dimension ref="A1:I44"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -535,157 +531,154 @@
       <c r="H1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="H2" s="2"/>
-      <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="H3" s="2"/>
-      <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="H4" s="2"/>
-      <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="H5" s="2"/>
-      <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="H6" s="2"/>
-      <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="H7" s="2"/>
-      <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="H8" s="2"/>
-      <c r="I8" s="1"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="H9" s="2"/>
-      <c r="I9" s="1"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="H10" s="2"/>
-      <c r="I10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="H11" s="2"/>
-      <c r="I11" s="1"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="H12" s="2"/>
-      <c r="I12" s="1"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="I13" s="1"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="I14" s="1"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="H15" s="2"/>
-      <c r="I15" s="1"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="I16" s="1"/>
-    </row>
-    <row r="17" spans="8:9" x14ac:dyDescent="0.3">
-      <c r="H17" s="2"/>
-      <c r="I17" s="1"/>
-    </row>
-    <row r="18" spans="8:9" x14ac:dyDescent="0.3">
-      <c r="I18" s="1"/>
-    </row>
-    <row r="19" spans="8:9" x14ac:dyDescent="0.3">
-      <c r="H19" s="2"/>
-      <c r="I19" s="1"/>
-    </row>
-    <row r="20" spans="8:9" x14ac:dyDescent="0.3">
-      <c r="I20" s="1"/>
-    </row>
-    <row r="21" spans="8:9" x14ac:dyDescent="0.3">
-      <c r="I21" s="1"/>
-    </row>
-    <row r="22" spans="8:9" x14ac:dyDescent="0.3">
-      <c r="I22" s="1"/>
-    </row>
-    <row r="23" spans="8:9" x14ac:dyDescent="0.3">
-      <c r="I23" s="1"/>
-    </row>
-    <row r="24" spans="8:9" x14ac:dyDescent="0.3">
-      <c r="H24" s="2"/>
-      <c r="I24" s="1"/>
-    </row>
-    <row r="25" spans="8:9" x14ac:dyDescent="0.3">
-      <c r="I25" s="1"/>
-    </row>
-    <row r="26" spans="8:9" x14ac:dyDescent="0.3">
-      <c r="H26" s="2"/>
-      <c r="I26" s="1"/>
-    </row>
-    <row r="27" spans="8:9" x14ac:dyDescent="0.3">
-      <c r="I27" s="1"/>
-    </row>
-    <row r="28" spans="8:9" x14ac:dyDescent="0.3">
-      <c r="H28" s="2"/>
-      <c r="I28" s="1"/>
-    </row>
-    <row r="29" spans="8:9" x14ac:dyDescent="0.3">
-      <c r="I29" s="1"/>
-    </row>
-    <row r="30" spans="8:9" x14ac:dyDescent="0.3">
-      <c r="H30" s="2"/>
-      <c r="I30" s="1"/>
-    </row>
-    <row r="31" spans="8:9" x14ac:dyDescent="0.3">
-      <c r="I31" s="1"/>
-    </row>
-    <row r="32" spans="8:9" x14ac:dyDescent="0.3">
-      <c r="I32" s="1"/>
-    </row>
-    <row r="33" spans="8:9" x14ac:dyDescent="0.3">
-      <c r="I33" s="1"/>
-    </row>
-    <row r="34" spans="8:9" x14ac:dyDescent="0.3">
-      <c r="I34" s="1"/>
-    </row>
-    <row r="35" spans="8:9" x14ac:dyDescent="0.3">
-      <c r="I35" s="1"/>
-    </row>
-    <row r="36" spans="8:9" x14ac:dyDescent="0.3">
-      <c r="I36" s="1"/>
-    </row>
-    <row r="37" spans="8:9" x14ac:dyDescent="0.3">
-      <c r="I37" s="1"/>
-    </row>
-    <row r="38" spans="8:9" x14ac:dyDescent="0.3">
-      <c r="H38" s="2"/>
-      <c r="I38" s="1"/>
-    </row>
-    <row r="39" spans="8:9" x14ac:dyDescent="0.3">
-      <c r="I39" s="1"/>
-    </row>
-    <row r="40" spans="8:9" x14ac:dyDescent="0.3">
-      <c r="I40" s="1"/>
-    </row>
-    <row r="41" spans="8:9" x14ac:dyDescent="0.3">
-      <c r="I41" s="1"/>
-    </row>
-    <row r="42" spans="8:9" x14ac:dyDescent="0.3">
-      <c r="I42" s="1"/>
-    </row>
-    <row r="43" spans="8:9" x14ac:dyDescent="0.3">
-      <c r="I43" s="1"/>
-    </row>
-    <row r="44" spans="8:9" x14ac:dyDescent="0.3">
-      <c r="I44" s="1"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G2" s="2"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G3" s="2"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G4" s="2"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G5" s="2"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G6" s="2"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G7" s="2"/>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G8" s="2"/>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G9" s="2"/>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G10" s="2"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G11" s="2"/>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G12" s="2"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G15" s="2"/>
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G17" s="2"/>
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G19" s="2"/>
+      <c r="H19" s="1"/>
+    </row>
+    <row r="20" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="H20" s="1"/>
+    </row>
+    <row r="21" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="H21" s="1"/>
+    </row>
+    <row r="22" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="H22" s="1"/>
+    </row>
+    <row r="23" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="H23" s="1"/>
+    </row>
+    <row r="24" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G24" s="2"/>
+      <c r="H24" s="1"/>
+    </row>
+    <row r="25" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="H25" s="1"/>
+    </row>
+    <row r="26" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G26" s="2"/>
+      <c r="H26" s="1"/>
+    </row>
+    <row r="27" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="H27" s="1"/>
+    </row>
+    <row r="28" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G28" s="2"/>
+      <c r="H28" s="1"/>
+    </row>
+    <row r="29" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="H29" s="1"/>
+    </row>
+    <row r="30" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G30" s="2"/>
+      <c r="H30" s="1"/>
+    </row>
+    <row r="31" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="H31" s="1"/>
+    </row>
+    <row r="32" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="H32" s="1"/>
+    </row>
+    <row r="33" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="H33" s="1"/>
+    </row>
+    <row r="34" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="H34" s="1"/>
+    </row>
+    <row r="35" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="H35" s="1"/>
+    </row>
+    <row r="36" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="H36" s="1"/>
+    </row>
+    <row r="37" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="H37" s="1"/>
+    </row>
+    <row r="38" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G38" s="2"/>
+      <c r="H38" s="1"/>
+    </row>
+    <row r="39" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="H39" s="1"/>
+    </row>
+    <row r="40" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="H40" s="1"/>
+    </row>
+    <row r="41" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="H41" s="1"/>
+    </row>
+    <row r="42" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="H42" s="1"/>
+    </row>
+    <row r="43" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="H43" s="1"/>
+    </row>
+    <row r="44" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="H44" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -696,8 +689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31C8FA34-854C-4FDF-A76D-37677D1C3B05}">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -711,13 +704,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D1" s="5"/>
     </row>

</xml_diff>